<commit_message>
Implemntação de Lista de Logs e alteerações no modo automático
</commit_message>
<xml_diff>
--- a/Programação Compra_Venda Semanal.xlsx
+++ b/Programação Compra_Venda Semanal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b61cfbbb06cf3b8/Documentos/Renda Extra/CapitalTrack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{45195C55-8BC5-4748-9132-C7950FDF4EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87CE04CC-DF14-F746-935A-50B9CA555D47}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{45195C55-8BC5-4748-9132-C7950FDF4EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C6803A3-673C-8046-B80A-A587F86056B4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{56232796-C73C-4DC9-A02A-F8E302482441}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -382,19 +382,19 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="XLNext Device" refreshedDate="45344.511448611112" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="33" xr:uid="{BE6C9250-E1CF-4E19-B4A7-4F77DD97E187}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="XLNext Device" refreshedDate="45352.799400462965" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{BE6C9250-E1CF-4E19-B4A7-4F77DD97E187}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela1"/>
   </cacheSource>
-  <cacheFields count="12">
+  <cacheFields count="13">
     <cacheField name="ID" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="33"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="39"/>
     </cacheField>
     <cacheField name="Simbolo" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="Data" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-09-13T00:00:00" maxDate="2024-02-22T00:00:00" count="21">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-09-13T00:00:00" maxDate="2024-03-24T00:00:00" count="24">
         <d v="2023-09-13T00:00:00"/>
         <d v="2023-09-15T00:00:00"/>
         <d v="2023-09-19T00:00:00"/>
@@ -416,14 +416,20 @@
         <d v="2024-02-14T00:00:00"/>
         <d v="2024-02-16T00:00:00"/>
         <d v="2024-02-21T00:00:00"/>
+        <d v="2024-02-22T00:00:00"/>
+        <d v="2024-02-23T00:00:00"/>
+        <d v="2024-03-23T00:00:00"/>
       </sharedItems>
-      <fieldGroup par="11"/>
+      <fieldGroup par="12"/>
     </cacheField>
     <cacheField name="QTD" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.99831999999999999" maxValue="11"/>
     </cacheField>
     <cacheField name="Valor de Compra" numFmtId="44">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.1499999999999999" maxValue="100.45"/>
+    </cacheField>
+    <cacheField name="Data da Venda" numFmtId="0">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-02-13T00:00:00" maxDate="2024-03-02T00:00:00"/>
     </cacheField>
     <cacheField name="Valor de Venda" numFmtId="44">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.1200000000000001" maxValue="96.11"/>
@@ -443,7 +449,7 @@
     </cacheField>
     <cacheField name="Meses (Data)" numFmtId="0" databaseField="0">
       <fieldGroup base="2">
-        <rangePr groupBy="months" startDate="2023-09-13T00:00:00" endDate="2024-02-22T00:00:00"/>
+        <rangePr groupBy="months" startDate="2023-09-13T00:00:00" endDate="2024-03-24T00:00:00"/>
         <groupItems count="14">
           <s v="&lt;13/09/2023"/>
           <s v="jan"/>
@@ -458,31 +464,31 @@
           <s v="out"/>
           <s v="nov"/>
           <s v="dez"/>
-          <s v="&gt;22/02/2024"/>
+          <s v="&gt;24/03/2024"/>
         </groupItems>
       </fieldGroup>
     </cacheField>
     <cacheField name="Trimestres (Data)" numFmtId="0" databaseField="0">
       <fieldGroup base="2">
-        <rangePr groupBy="quarters" startDate="2023-09-13T00:00:00" endDate="2024-02-22T00:00:00"/>
+        <rangePr groupBy="quarters" startDate="2023-09-13T00:00:00" endDate="2024-03-24T00:00:00"/>
         <groupItems count="6">
           <s v="&lt;13/09/2023"/>
           <s v="Trim1"/>
           <s v="Trim2"/>
           <s v="Trim3"/>
           <s v="Trim4"/>
-          <s v="&gt;22/02/2024"/>
+          <s v="&gt;24/03/2024"/>
         </groupItems>
       </fieldGroup>
     </cacheField>
     <cacheField name="Anos (Data)" numFmtId="0" databaseField="0">
       <fieldGroup base="2">
-        <rangePr groupBy="years" startDate="2023-09-13T00:00:00" endDate="2024-02-22T00:00:00"/>
+        <rangePr groupBy="years" startDate="2023-09-13T00:00:00" endDate="2024-03-24T00:00:00"/>
         <groupItems count="4">
           <s v="&lt;13/09/2023"/>
           <s v="2023"/>
           <s v="2024"/>
-          <s v="&gt;22/02/2024"/>
+          <s v="&gt;24/03/2024"/>
         </groupItems>
       </fieldGroup>
     </cacheField>
@@ -496,13 +502,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="33">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="39">
   <r>
     <n v="1"/>
     <s v="TMF"/>
     <x v="0"/>
     <n v="0.99831999999999999"/>
     <n v="5.96"/>
+    <m/>
     <n v="5.25"/>
     <n v="-0.71"/>
     <n v="-0.70880719999999997"/>
@@ -514,6 +521,7 @@
     <x v="0"/>
     <n v="1.0002"/>
     <n v="58.62"/>
+    <m/>
     <n v="58.65"/>
     <n v="3.0000000000001137E-2"/>
     <n v="3.0006000000001136E-2"/>
@@ -525,6 +533,7 @@
     <x v="0"/>
     <n v="0.99936000000000003"/>
     <n v="12.73"/>
+    <m/>
     <n v="12.92"/>
     <n v="0.1899999999999995"/>
     <n v="0.1898783999999995"/>
@@ -536,6 +545,7 @@
     <x v="1"/>
     <n v="1"/>
     <n v="12.23"/>
+    <m/>
     <n v="13.15"/>
     <n v="0.91999999999999993"/>
     <n v="0.91999999999999993"/>
@@ -547,6 +557,7 @@
     <x v="2"/>
     <n v="1"/>
     <n v="4.1500000000000004"/>
+    <m/>
     <n v="4.1399999999999997"/>
     <n v="-1.0000000000000675E-2"/>
     <n v="-1.0000000000000675E-2"/>
@@ -558,6 +569,7 @@
     <x v="3"/>
     <n v="1"/>
     <n v="11.7"/>
+    <m/>
     <n v="13.15"/>
     <n v="1.4500000000000011"/>
     <n v="1.4500000000000011"/>
@@ -569,6 +581,7 @@
     <x v="3"/>
     <n v="1"/>
     <n v="5.3"/>
+    <m/>
     <n v="5.15"/>
     <n v="-0.14999999999999947"/>
     <n v="-0.14999999999999947"/>
@@ -580,6 +593,7 @@
     <x v="4"/>
     <n v="1"/>
     <n v="4.6399999999999997"/>
+    <m/>
     <n v="5.15"/>
     <n v="0.51000000000000068"/>
     <n v="0.51000000000000068"/>
@@ -591,6 +605,7 @@
     <x v="4"/>
     <n v="1"/>
     <n v="11.59"/>
+    <m/>
     <n v="13.15"/>
     <n v="1.5600000000000005"/>
     <n v="1.5600000000000005"/>
@@ -602,6 +617,7 @@
     <x v="4"/>
     <n v="2"/>
     <n v="10.54"/>
+    <m/>
     <n v="10.54"/>
     <n v="0"/>
     <n v="0"/>
@@ -613,6 +629,7 @@
     <x v="5"/>
     <n v="1"/>
     <n v="4.42"/>
+    <m/>
     <n v="5.15"/>
     <n v="0.73000000000000043"/>
     <n v="0.73000000000000043"/>
@@ -624,6 +641,7 @@
     <x v="6"/>
     <n v="1"/>
     <n v="89.54"/>
+    <m/>
     <n v="96.11"/>
     <n v="6.5699999999999932"/>
     <n v="6.5699999999999932"/>
@@ -635,6 +653,7 @@
     <x v="7"/>
     <n v="10"/>
     <n v="1.1499999999999999"/>
+    <m/>
     <n v="1.1200000000000001"/>
     <n v="-2.9999999999999805E-2"/>
     <n v="-0.29999999999999805"/>
@@ -646,6 +665,7 @@
     <x v="8"/>
     <n v="1"/>
     <n v="57"/>
+    <m/>
     <n v="58.65"/>
     <n v="1.6499999999999986"/>
     <n v="1.6499999999999986"/>
@@ -657,6 +677,7 @@
     <x v="9"/>
     <n v="1"/>
     <n v="11.99"/>
+    <m/>
     <n v="13.15"/>
     <n v="1.1600000000000001"/>
     <n v="1.1600000000000001"/>
@@ -668,6 +689,7 @@
     <x v="10"/>
     <n v="2"/>
     <n v="58.54"/>
+    <m/>
     <n v="58.65"/>
     <n v="0.10999999999999943"/>
     <n v="0.21999999999999886"/>
@@ -679,6 +701,7 @@
     <x v="11"/>
     <n v="1"/>
     <n v="100.45"/>
+    <m/>
     <n v="91.36"/>
     <n v="-9.0900000000000034"/>
     <n v="-9.0900000000000034"/>
@@ -690,6 +713,7 @@
     <x v="12"/>
     <n v="5"/>
     <n v="12.4"/>
+    <m/>
     <n v="12.8"/>
     <n v="0.40000000000000036"/>
     <n v="2.0000000000000018"/>
@@ -701,6 +725,7 @@
     <x v="12"/>
     <n v="5"/>
     <n v="18.329999999999998"/>
+    <m/>
     <n v="18.649999999999999"/>
     <n v="0.32000000000000028"/>
     <n v="1.6000000000000014"/>
@@ -712,6 +737,7 @@
     <x v="13"/>
     <n v="3"/>
     <n v="13.45"/>
+    <m/>
     <n v="14.65"/>
     <n v="1.2000000000000011"/>
     <n v="3.6000000000000032"/>
@@ -723,6 +749,7 @@
     <x v="14"/>
     <n v="10"/>
     <n v="4.5599999999999996"/>
+    <m/>
     <n v="4.33"/>
     <n v="-0.22999999999999954"/>
     <n v="-2.2999999999999954"/>
@@ -734,6 +761,7 @@
     <x v="14"/>
     <n v="10"/>
     <n v="14.31"/>
+    <m/>
     <n v="13.96"/>
     <n v="-0.34999999999999964"/>
     <n v="-3.4999999999999964"/>
@@ -745,6 +773,7 @@
     <x v="15"/>
     <n v="5"/>
     <n v="12.9"/>
+    <m/>
     <n v="13.51"/>
     <n v="0.60999999999999943"/>
     <n v="3.0499999999999972"/>
@@ -756,6 +785,7 @@
     <x v="16"/>
     <n v="1"/>
     <n v="76.66"/>
+    <m/>
     <n v="78.83"/>
     <n v="2.1700000000000017"/>
     <n v="2.1700000000000017"/>
@@ -767,6 +797,7 @@
     <x v="16"/>
     <n v="3"/>
     <n v="18.89"/>
+    <m/>
     <n v="18.059999999999999"/>
     <n v="-0.83000000000000185"/>
     <n v="-2.4900000000000055"/>
@@ -778,6 +809,7 @@
     <x v="17"/>
     <n v="3"/>
     <n v="16.079999999999998"/>
+    <m/>
     <n v="15.42"/>
     <n v="-0.65999999999999837"/>
     <n v="-1.9799999999999951"/>
@@ -789,6 +821,7 @@
     <x v="18"/>
     <n v="5"/>
     <n v="7.36"/>
+    <m/>
     <n v="7.37"/>
     <n v="9.9999999999997868E-3"/>
     <n v="4.9999999999998934E-2"/>
@@ -800,6 +833,7 @@
     <x v="18"/>
     <n v="2"/>
     <n v="75"/>
+    <m/>
     <n v="73.63"/>
     <n v="-1.3700000000000045"/>
     <n v="-2.7400000000000091"/>
@@ -811,6 +845,7 @@
     <x v="19"/>
     <n v="11"/>
     <n v="7.4"/>
+    <m/>
     <n v="7.37"/>
     <n v="-3.0000000000000249E-2"/>
     <n v="-0.33000000000000274"/>
@@ -822,6 +857,7 @@
     <x v="19"/>
     <n v="10"/>
     <n v="10.96"/>
+    <m/>
     <n v="10.16"/>
     <n v="-0.80000000000000071"/>
     <n v="-8.0000000000000071"/>
@@ -833,10 +869,11 @@
     <x v="20"/>
     <n v="6"/>
     <n v="13.96"/>
-    <m/>
-    <s v="Trade Aberto"/>
-    <s v=""/>
-    <x v="2"/>
+    <d v="2024-02-13T00:00:00"/>
+    <n v="13.94"/>
+    <n v="-2.000000000000135E-2"/>
+    <n v="-0.1200000000000081"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="32"/>
@@ -844,10 +881,11 @@
     <x v="20"/>
     <n v="2"/>
     <n v="24.13"/>
-    <m/>
-    <s v="Trade Aberto"/>
-    <s v=""/>
-    <x v="2"/>
+    <d v="2024-02-27T00:00:00"/>
+    <n v="24.08"/>
+    <n v="-5.0000000000000711E-2"/>
+    <n v="-0.10000000000000142"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="33"/>
@@ -856,6 +894,79 @@
     <n v="1"/>
     <n v="19.07"/>
     <m/>
+    <m/>
+    <s v="Trade Aberto"/>
+    <s v=""/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="FGFPP"/>
+    <x v="21"/>
+    <n v="1"/>
+    <n v="18.2"/>
+    <d v="2024-02-29T00:00:00"/>
+    <n v="18.010000000000002"/>
+    <n v="-0.18999999999999773"/>
+    <n v="-0.18999999999999773"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="SLF"/>
+    <x v="21"/>
+    <n v="1"/>
+    <n v="54.36"/>
+    <m/>
+    <m/>
+    <s v="Trade Aberto"/>
+    <s v=""/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="ABR"/>
+    <x v="22"/>
+    <n v="2"/>
+    <n v="12.85"/>
+    <d v="2024-03-01T00:00:00"/>
+    <n v="12.9"/>
+    <n v="5.0000000000000711E-2"/>
+    <n v="0.10000000000000142"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <s v="FGFPP"/>
+    <x v="22"/>
+    <n v="1"/>
+    <n v="18.100000000000001"/>
+    <d v="2024-02-29T00:00:00"/>
+    <n v="18.010000000000002"/>
+    <n v="-8.9999999999999858E-2"/>
+    <n v="-8.9999999999999858E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="ABR"/>
+    <x v="22"/>
+    <n v="2"/>
+    <n v="12.85"/>
+    <d v="2024-03-01T00:00:00"/>
+    <n v="12.9"/>
+    <n v="5.0000000000000711E-2"/>
+    <n v="0.10000000000000142"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="SLF"/>
+    <x v="23"/>
+    <n v="1"/>
+    <n v="54.97"/>
+    <m/>
+    <m/>
     <s v="Trade Aberto"/>
     <s v=""/>
     <x v="2"/>
@@ -864,13 +975,13 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADADC71A-AF86-414C-9EBF-9D9BAE83197F}" name="Tabela dinâmica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H4:I7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50BF2D8E-F21F-41F5-9782-417585B77C95}" name="Tabela dinâmica1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B4:C7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="22">
+      <items count="25">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -892,9 +1003,254 @@
         <item x="18"/>
         <item x="19"/>
         <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="12"/>
+    <field x="11"/>
+    <field x="10"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Ganho Total" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{479F3482-A03B-464C-86FD-0A406D39A63A}" name="Tabela dinâmica4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J4:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="25">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="12"/>
+    <field x="11"/>
+    <field x="10"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="9" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Contagem de Acerto" fld="9" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADADC71A-AF86-414C-9EBF-9D9BAE83197F}" name="Tabela dinâmica3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H4:I7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="25">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -946,9 +1302,9 @@
     </pivotField>
   </pivotFields>
   <rowFields count="4">
+    <field x="12"/>
     <field x="11"/>
     <field x="10"/>
-    <field x="9"/>
     <field x="2"/>
   </rowFields>
   <rowItems count="3">
@@ -966,10 +1322,10 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="8" hier="-1"/>
+    <pageField fld="9" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Contagem de Acerto" fld="8" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Contagem de Acerto" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -983,14 +1339,14 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{645885E9-FACE-4AD3-873C-DA1B8733D2DE}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{645885E9-FACE-4AD3-873C-DA1B8733D2DE}" name="Tabela dinâmica2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E4:F7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="12">
+  <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="22">
+      <items count="25">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1012,9 +1368,13 @@
         <item x="18"/>
         <item x="19"/>
         <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1066,9 +1426,9 @@
     </pivotField>
   </pivotFields>
   <rowFields count="4">
+    <field x="12"/>
     <field x="11"/>
     <field x="10"/>
-    <field x="9"/>
     <field x="2"/>
   </rowFields>
   <rowItems count="3">
@@ -1086,243 +1446,10 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="8" hier="-1"/>
+    <pageField fld="9" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Contagem de Acerto" fld="8" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{50BF2D8E-F21F-41F5-9782-417585B77C95}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B4:C7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="22">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="11"/>
-    <field x="10"/>
-    <field x="9"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de Ganho Total" fld="7" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{479F3482-A03B-464C-86FD-0A406D39A63A}" name="Tabela dinâmica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="J4:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="12">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="22">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item h="1" x="2"/>
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="11"/>
-    <field x="10"/>
-    <field x="9"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="8" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Contagem de Acerto" fld="8" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Contagem de Acerto" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1680,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC3AB56-FD96-4B02-86AA-B5205E9477E7}">
   <dimension ref="A2:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2043,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4ECBE7-48CD-46F2-AAD9-8A52FDAC5D23}">
   <dimension ref="B2:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="E27" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3132,18 +3259,23 @@
       <c r="F34" s="9">
         <v>24.13</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="I34" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
-        <v>Trade Aberto</v>
-      </c>
-      <c r="J34" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
-        <v/>
+      <c r="G34" s="5">
+        <v>45349</v>
+      </c>
+      <c r="H34" s="9">
+        <v>24.08</v>
+      </c>
+      <c r="I34" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
+        <v>-5.0000000000000711E-2</v>
+      </c>
+      <c r="J34" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
+        <v>-0.10000000000000142</v>
       </c>
       <c r="K34" t="str">
         <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","",IF(Tabela1[[#This Row],[Ganho Total]]&gt;0,"S","N"))</f>
-        <v/>
+        <v>N</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
@@ -3192,18 +3324,23 @@
       <c r="F36" s="9">
         <v>18.2</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="I36" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
-        <v>Trade Aberto</v>
-      </c>
-      <c r="J36" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
-        <v/>
+      <c r="G36" s="5">
+        <v>45351</v>
+      </c>
+      <c r="H36" s="9">
+        <v>18.010000000000002</v>
+      </c>
+      <c r="I36" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
+        <v>-0.18999999999999773</v>
+      </c>
+      <c r="J36" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
+        <v>-0.18999999999999773</v>
       </c>
       <c r="K36" t="str">
         <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","",IF(Tabela1[[#This Row],[Ganho Total]]&gt;0,"S","N"))</f>
-        <v/>
+        <v>N</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
@@ -3252,18 +3389,23 @@
       <c r="F38" s="9">
         <v>12.85</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="I38" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
-        <v>Trade Aberto</v>
-      </c>
-      <c r="J38" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
-        <v/>
+      <c r="G38" s="5">
+        <v>45352</v>
+      </c>
+      <c r="H38" s="9">
+        <v>12.9</v>
+      </c>
+      <c r="I38" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
+        <v>5.0000000000000711E-2</v>
+      </c>
+      <c r="J38" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
+        <v>0.10000000000000142</v>
       </c>
       <c r="K38" s="10" t="str">
         <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","",IF(Tabela1[[#This Row],[Ganho Total]]&gt;0,"S","N"))</f>
-        <v/>
+        <v>S</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -3282,18 +3424,23 @@
       <c r="F39" s="9">
         <v>18.100000000000001</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="I39" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
-        <v>Trade Aberto</v>
-      </c>
-      <c r="J39" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
-        <v/>
+      <c r="G39" s="5">
+        <v>45351</v>
+      </c>
+      <c r="H39" s="9">
+        <v>18.010000000000002</v>
+      </c>
+      <c r="I39" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
+        <v>-8.9999999999999858E-2</v>
+      </c>
+      <c r="J39" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
+        <v>-8.9999999999999858E-2</v>
       </c>
       <c r="K39" s="10" t="str">
         <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","",IF(Tabela1[[#This Row],[Ganho Total]]&gt;0,"S","N"))</f>
-        <v/>
+        <v>N</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -3312,18 +3459,23 @@
       <c r="F40" s="9">
         <v>12.85</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="I40" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
-        <v>Trade Aberto</v>
-      </c>
-      <c r="J40" s="9" t="str">
-        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
-        <v/>
+      <c r="G40" s="5">
+        <v>45352</v>
+      </c>
+      <c r="H40" s="9">
+        <v>12.9</v>
+      </c>
+      <c r="I40" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","Trade Aberto",Tabela1[[#This Row],[Valor de Venda]]-Tabela1[[#This Row],[Valor de Compra]])</f>
+        <v>5.0000000000000711E-2</v>
+      </c>
+      <c r="J40" s="9">
+        <f>IF(Tabela1[[#This Row],[Valor de Venda]]="", "",Tabela1[[#This Row],[Ganho Por Ação]]*Tabela1[[#This Row],[QTD]])</f>
+        <v>0.10000000000000142</v>
       </c>
       <c r="K40" s="10" t="str">
         <f>IF(Tabela1[[#This Row],[Valor de Venda]]="","",IF(Tabela1[[#This Row],[Ganho Total]]&gt;0,"S","N"))</f>
-        <v/>
+        <v>S</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -3369,7 +3521,7 @@
   <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3434,13 +3586,13 @@
       <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>4.7310771999999943</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="10">
         <v>17</v>
       </c>
       <c r="G5" s="8">
@@ -3450,13 +3602,13 @@
       <c r="H5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="10">
         <v>11</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="10">
         <v>6</v>
       </c>
     </row>
@@ -3464,56 +3616,56 @@
       <c r="B6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C6">
-        <v>-8.8700000000000081</v>
+      <c r="C6" s="10">
+        <v>-9.1700000000000124</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F6">
-        <v>13</v>
+      <c r="F6" s="10">
+        <v>19</v>
       </c>
       <c r="G6" s="8">
         <f>GETPIVOTDATA("Acerto",$H$4,"Anos (Data)",2024)/GETPIVOTDATA("Acerto",$E$4,"Anos (Data)",2024)</f>
-        <v>0.46153846153846156</v>
+        <v>0.42105263157894735</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I6">
-        <v>6</v>
+      <c r="I6" s="10">
+        <v>8</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K6">
-        <v>7</v>
+      <c r="K6" s="10">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C7">
-        <v>-4.1389228000000138</v>
+      <c r="C7" s="10">
+        <v>-4.438922800000018</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F7">
-        <v>30</v>
+      <c r="F7" s="10">
+        <v>36</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I7">
-        <v>17</v>
+      <c r="I7" s="10">
+        <v>19</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K7">
-        <v>13</v>
+      <c r="K7" s="10">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>